<commit_message>
Finished Comparison of Not bio to Bio
</commit_message>
<xml_diff>
--- a/most_bought_nonorg.xlsx
+++ b/most_bought_nonorg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FHNW\zR\Warenkorbanalyse\warenkorbanalyse_fhnw_ds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EA9BF8-6D44-44C6-8D1E-4F3A188524F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B453030-C154-4931-AA70-4B88947A2F56}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5329" uniqueCount="5165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5897" uniqueCount="5170">
   <si>
     <t>product_name</t>
   </si>
@@ -15473,9 +15473,6 @@
     <t>Recycled Paper Towels</t>
   </si>
   <si>
-    <t>Turkey Breast</t>
-  </si>
-  <si>
     <t>Orange Juice</t>
   </si>
   <si>
@@ -15527,14 +15524,32 @@
     <t>Total Bio</t>
   </si>
   <si>
-    <t>None</t>
+    <t>Black Beans</t>
+  </si>
+  <si>
+    <t>Sehe zeile 24</t>
+  </si>
+  <si>
+    <t>Organic Red Pepper (unklear if red pepper or red pepper)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legende: </t>
+  </si>
+  <si>
+    <t>Needs attention/review</t>
+  </si>
+  <si>
+    <t>Simliar product BUT NOT SAME, NEED SECOND OPINION</t>
+  </si>
+  <si>
+    <t>No equivalent Bioproduct found</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -15547,13 +15562,39 @@
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -15568,7 +15609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -15583,6 +15624,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15879,15 +15939,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U101"/>
+  <dimension ref="A1:U107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="44.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.47265625" style="3" customWidth="1"/>
     <col min="3" max="3" width="41.3671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.62890625" customWidth="1"/>
@@ -15928,7 +15988,7 @@
         <v>5140</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>5163</v>
+        <v>5162</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -15957,7 +16017,7 @@
         <v>20915</v>
       </c>
       <c r="H2" t="s">
-        <v>5159</v>
+        <v>5158</v>
       </c>
       <c r="I2" s="4">
         <f>'Sheet 2'!$C$1356</f>
@@ -15982,17 +16042,17 @@
         <f t="shared" si="0"/>
         <v>91277</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="6" t="s">
         <v>5120</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <f>'Sheet 2'!$C$19</f>
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="6" t="s">
         <v>4559</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="6">
         <f>'Sheet 2'!$C$580</f>
         <v>91251</v>
       </c>
@@ -16081,31 +16141,31 @@
         <f t="shared" si="0"/>
         <v>118908</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="6" t="s">
         <v>4779</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <f>'Sheet 2'!C360</f>
         <v>39</v>
       </c>
-      <c r="H6" t="s">
-        <v>5160</v>
-      </c>
-      <c r="I6">
+      <c r="H6" s="6" t="s">
+        <v>5159</v>
+      </c>
+      <c r="I6" s="6">
         <f>'Sheet 2'!C1053+'Sheet 2'!C2175</f>
         <v>8808</v>
       </c>
-      <c r="J6" t="s">
-        <v>5161</v>
-      </c>
-      <c r="K6">
+      <c r="J6" s="6" t="s">
+        <v>5160</v>
+      </c>
+      <c r="K6" s="6">
         <f>'Sheet 2'!C1291+'Sheet 2'!C3125</f>
         <v>85243</v>
       </c>
-      <c r="L6" t="s">
-        <v>5162</v>
-      </c>
-      <c r="M6">
+      <c r="L6" s="6" t="s">
+        <v>5161</v>
+      </c>
+      <c r="M6" s="6">
         <f>'Sheet 2'!C3749</f>
         <v>24818</v>
       </c>
@@ -16118,7 +16178,7 @@
         <v>86748</v>
       </c>
       <c r="C7" t="s">
-        <v>5153</v>
+        <v>5152</v>
       </c>
       <c r="D7" s="1" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C7,'Sheet 2'!B:B)))&gt;0</f>
@@ -16162,21 +16222,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
-      <c r="A9" t="s">
+    <row r="9" spans="1:21" s="9" customFormat="1">
+      <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="10">
         <v>79245</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="9" t="s">
         <v>5142</v>
       </c>
-      <c r="D9" s="1" t="b">
+      <c r="D9" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C9,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -16477,38 +16537,31 @@
       </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>142990</v>
+        <v>142603</v>
       </c>
       <c r="F17" t="s">
-        <v>2662</v>
+        <v>2258</v>
       </c>
       <c r="G17">
-        <f>'Sheet 2'!C2477</f>
-        <v>387</v>
-      </c>
-      <c r="H17" t="s">
-        <v>2258</v>
-      </c>
-      <c r="I17">
         <f>'Sheet 2'!C2881</f>
         <v>142603</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
-      <c r="A18" t="s">
+    <row r="18" spans="1:17" s="9" customFormat="1">
+      <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="10">
         <v>58312</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="1" t="b">
+      <c r="D18" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C18,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -16574,26 +16627,30 @@
         <v>105026</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
-      <c r="A20" t="s">
+    <row r="20" spans="1:17" s="9" customFormat="1">
+      <c r="A20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="10">
         <v>58185</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="1" t="b">
+      <c r="D20" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C20,'Sheet 2'!B:B)))&gt;0</f>
         <v>1</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>5164</v>
+        <v>14</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>5165</v>
+      </c>
+      <c r="G20" s="7">
+        <f>'Sheet 2'!C363</f>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -16680,10 +16737,10 @@
         <f>'Sheet 2'!C4802</f>
         <v>220877</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="6" t="s">
         <v>1165</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="6">
         <f>'Sheet 2'!C3974</f>
         <v>2925</v>
       </c>
@@ -16710,14 +16767,14 @@
         <v>3335</v>
       </c>
       <c r="G24">
-        <f>'Sheet 2'!C1804</f>
+        <f>'Sheet 2'!$C$1804</f>
         <v>17462</v>
       </c>
       <c r="H24" t="s">
         <v>3280</v>
       </c>
       <c r="I24">
-        <f>'Sheet 2'!C1859</f>
+        <f>'Sheet 2'!$C$1859</f>
         <v>351</v>
       </c>
     </row>
@@ -16768,59 +16825,59 @@
         <v>13836</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="A26" t="s">
+    <row r="26" spans="1:17" s="9" customFormat="1">
+      <c r="A26" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="10">
         <v>52124</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="1" t="b">
+      <c r="D26" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C26,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
-      <c r="A27" t="s">
+    <row r="27" spans="1:17" s="9" customFormat="1">
+      <c r="A27" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="10">
         <v>51738</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="1" t="b">
+      <c r="D27" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C27,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
-      <c r="A28" t="s">
+    <row r="28" spans="1:17" s="9" customFormat="1">
+      <c r="A28" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="10">
         <v>48512</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="1" t="b">
+      <c r="D28" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C28,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -16869,10 +16926,10 @@
         <f t="shared" si="0"/>
         <v>1893</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="6" t="s">
         <v>1648</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="6">
         <f>'Sheet 2'!C3491</f>
         <v>1893</v>
       </c>
@@ -16910,21 +16967,21 @@
         <v>6226</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
-      <c r="A32" t="s">
+    <row r="32" spans="1:17" s="9" customFormat="1">
+      <c r="A32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="10">
         <v>44737</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="9" t="s">
         <v>5143</v>
       </c>
-      <c r="D32" s="1" t="b">
+      <c r="D32" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C32,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -16955,40 +17012,40 @@
         <v>70804</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
-      <c r="A34" t="s">
+    <row r="34" spans="1:11" s="9" customFormat="1">
+      <c r="A34" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="10">
         <v>44460</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="1" t="b">
+      <c r="D34" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C34,'Sheet 2'!B:B)))&gt;0</f>
         <v>1</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
+    <row r="35" spans="1:11" s="9" customFormat="1">
+      <c r="A35" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="10">
         <v>43261</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="1" t="b">
+      <c r="D35" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C35,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17001,7 +17058,7 @@
         <v>42274</v>
       </c>
       <c r="C36" t="s">
-        <v>5154</v>
+        <v>5153</v>
       </c>
       <c r="D36" s="1" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C36,'Sheet 2'!B:B)))&gt;0</f>
@@ -17059,21 +17116,21 @@
         <v>30517</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
-      <c r="A38" t="s">
+    <row r="38" spans="1:11" s="9" customFormat="1">
+      <c r="A38" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="10">
         <v>41303</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="1" t="b">
+      <c r="D38" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C38,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17122,10 +17179,10 @@
         <f t="shared" si="0"/>
         <v>22335</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="6" t="s">
         <v>1185</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="6">
         <f>'Sheet 2'!C3954</f>
         <v>22335</v>
       </c>
@@ -17138,7 +17195,7 @@
         <v>39271</v>
       </c>
       <c r="C41" t="s">
-        <v>5155</v>
+        <v>5154</v>
       </c>
       <c r="D41" s="1" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C41,'Sheet 2'!B:B)))&gt;0</f>
@@ -17181,10 +17238,10 @@
         <f>'Sheet 2'!C186</f>
         <v>24175</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="6" t="s">
         <v>3157</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="6">
         <f>'Sheet 2'!C1982</f>
         <v>1861</v>
       </c>
@@ -17274,21 +17331,21 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
-      <c r="A46" t="s">
+    <row r="46" spans="1:11" s="9" customFormat="1">
+      <c r="A46" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="10">
         <v>37298</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="1" t="b">
+      <c r="D46" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C46,'Sheet 2'!B:B)))&gt;0</f>
         <v>1</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17385,59 +17442,59 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
-      <c r="A50" t="s">
+    <row r="50" spans="1:11" s="9" customFormat="1">
+      <c r="A50" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="10">
         <v>36048</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="1" t="b">
+      <c r="D50" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C50,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
-      <c r="A51" t="s">
+    <row r="51" spans="1:11" s="9" customFormat="1">
+      <c r="A51" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="10">
         <v>35384</v>
       </c>
-      <c r="C51" t="s">
-        <v>5156</v>
-      </c>
-      <c r="D51" s="1" t="b">
+      <c r="C51" s="9" t="s">
+        <v>5155</v>
+      </c>
+      <c r="D51" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C51,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
-      <c r="A52" t="s">
+    <row r="52" spans="1:11" s="9" customFormat="1">
+      <c r="A52" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="10">
         <v>34211</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="1" t="b">
+      <c r="D52" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C52,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17468,40 +17525,40 @@
         <v>196</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
-      <c r="A54" t="s">
+    <row r="54" spans="1:11" s="9" customFormat="1">
+      <c r="A54" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="10">
         <v>32270</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="1" t="b">
+      <c r="D54" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C54,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
-      <c r="A55" t="s">
+    <row r="55" spans="1:11" s="9" customFormat="1">
+      <c r="A55" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="10">
         <v>32212</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="1" t="b">
+      <c r="D55" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C55,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17532,21 +17589,21 @@
         <v>224</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
-      <c r="A57" t="s">
+    <row r="57" spans="1:11" s="9" customFormat="1">
+      <c r="A57" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="10">
         <v>32069</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="9" t="s">
         <v>5143</v>
       </c>
-      <c r="D57" s="1" t="b">
+      <c r="D57" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C57,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17584,21 +17641,21 @@
         <v>4331</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
-      <c r="A59" t="s">
+    <row r="59" spans="1:11" s="9" customFormat="1">
+      <c r="A59" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="10">
         <v>30866</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="9" t="s">
         <v>5144</v>
       </c>
-      <c r="D59" s="1" t="b">
+      <c r="D59" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C59,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E59" s="5">
+      <c r="E59" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17659,7 +17716,21 @@
       </c>
       <c r="E61" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>28458</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1457</v>
+      </c>
+      <c r="G61">
+        <f>'Sheet 2'!C3682</f>
+        <v>27402</v>
+      </c>
+      <c r="H61" t="s">
+        <v>1097</v>
+      </c>
+      <c r="I61">
+        <f>'Sheet 2'!C4042</f>
+        <v>1056</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -17678,24 +17749,38 @@
       </c>
       <c r="E62" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="A63" t="s">
+        <v>7193</v>
+      </c>
+      <c r="F62" t="s">
+        <v>3567</v>
+      </c>
+      <c r="G62">
+        <f>'Sheet 2'!C1572</f>
+        <v>7076</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>4056</v>
+      </c>
+      <c r="I62" s="6">
+        <f>'Sheet 2'!C1083</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="9" customFormat="1">
+      <c r="A63" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="10">
         <v>30009</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="1" t="b">
+      <c r="D63" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C63,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E63" s="5">
+      <c r="E63" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -17708,37 +17793,44 @@
         <v>29174</v>
       </c>
       <c r="C64" t="s">
-        <v>64</v>
+        <v>5163</v>
       </c>
       <c r="D64" s="1" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C64,'Sheet 2'!B:B)))&gt;0</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" t="s">
+        <v>39577</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>2356</v>
+      </c>
+      <c r="G64" s="6">
+        <f>'Sheet 2'!C2783</f>
+        <v>39577</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" s="9" customFormat="1">
+      <c r="A65" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="10">
         <v>29047</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="9" t="s">
         <v>5145</v>
       </c>
-      <c r="D65" s="1" t="b">
+      <c r="D65" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C65,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E65" s="5">
+      <c r="E65" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:13">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -17754,10 +17846,17 @@
       </c>
       <c r="E66" s="5">
         <f t="shared" ref="E66:E101" si="1">G66++I66+K66+M66+O66+Q66+S66+U66</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>8391</v>
+      </c>
+      <c r="F66" t="s">
+        <v>4867</v>
+      </c>
+      <c r="G66">
+        <f>'Sheet 2'!C272</f>
+        <v>8391</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -17773,10 +17872,24 @@
       </c>
       <c r="E67" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>5442</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>2459</v>
+      </c>
+      <c r="G67" s="6">
+        <f>'Sheet 2'!C2680</f>
+        <v>5414</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="I67" s="6">
+        <f>'Sheet 2'!C4570</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -17784,7 +17897,7 @@
         <v>27871</v>
       </c>
       <c r="C68" t="s">
-        <v>5157</v>
+        <v>5156</v>
       </c>
       <c r="D68" s="1" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C68,'Sheet 2'!B:B)))&gt;0</f>
@@ -17792,29 +17905,36 @@
       </c>
       <c r="E68" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" t="s">
+        <v>1780</v>
+      </c>
+      <c r="F68" t="s">
+        <v>499</v>
+      </c>
+      <c r="G68">
+        <f>'Sheet 2'!C4640</f>
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" s="9" customFormat="1">
+      <c r="A69" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="10">
         <v>27813</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D69" s="1" t="b">
+      <c r="D69" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C69,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E69" s="5">
+      <c r="E69" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:13">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -17830,10 +17950,17 @@
       </c>
       <c r="E70" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+        <v>387</v>
+      </c>
+      <c r="F70" t="s">
+        <v>2662</v>
+      </c>
+      <c r="G70">
+        <f>'Sheet 2'!C2477</f>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -17841,18 +17968,18 @@
         <v>27679</v>
       </c>
       <c r="C71" t="s">
-        <v>5146</v>
+        <v>71</v>
       </c>
       <c r="D71" s="1" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C71,'Sheet 2'!B:B)))&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:13">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -17868,48 +17995,62 @@
       </c>
       <c r="E72" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" t="s">
+        <v>16974</v>
+      </c>
+      <c r="F72" t="s">
+        <v>3705</v>
+      </c>
+      <c r="G72">
+        <f>'Sheet 2'!C1434</f>
+        <v>16479</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>4072</v>
+      </c>
+      <c r="I72" s="6">
+        <f>'Sheet 2'!C1067</f>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="9" customFormat="1">
+      <c r="A73" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="10">
         <v>27394</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D73" s="1" t="b">
+      <c r="D73" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C73,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E73" s="5">
+      <c r="E73" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
-      <c r="A74" t="s">
+    <row r="74" spans="1:13" s="9" customFormat="1">
+      <c r="A74" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="10">
         <v>27200</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="1" t="b">
+      <c r="D74" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C74,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E74" s="5">
+      <c r="E74" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:13">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -17917,7 +18058,7 @@
         <v>26962</v>
       </c>
       <c r="C75" t="s">
-        <v>75</v>
+        <v>2611</v>
       </c>
       <c r="D75" s="1" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C75,'Sheet 2'!B:B)))&gt;0</f>
@@ -17925,29 +18066,43 @@
       </c>
       <c r="E75" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" t="s">
+        <v>13169</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>2611</v>
+      </c>
+      <c r="G75" s="6">
+        <f>'Sheet 2'!C2528</f>
+        <v>50</v>
+      </c>
+      <c r="H75" t="s">
+        <v>993</v>
+      </c>
+      <c r="I75">
+        <f>'Sheet 2'!C4146</f>
+        <v>13119</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" s="9" customFormat="1">
+      <c r="A76" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="10">
         <v>26625</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D76" s="1" t="b">
+      <c r="D76" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C76,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E76" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:13">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -17963,10 +18118,17 @@
       </c>
       <c r="E77" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+        <v>1739</v>
+      </c>
+      <c r="F77" t="s">
+        <v>4341</v>
+      </c>
+      <c r="G77">
+        <f>'Sheet 2'!C798</f>
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -17974,7 +18136,7 @@
         <v>25972</v>
       </c>
       <c r="C78" t="s">
-        <v>5147</v>
+        <v>5146</v>
       </c>
       <c r="D78" s="1" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C78,'Sheet 2'!B:B)))&gt;0</f>
@@ -17982,86 +18144,114 @@
       </c>
       <c r="E78" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" t="s">
+        <v>18890</v>
+      </c>
+      <c r="F78" t="s">
+        <v>1995</v>
+      </c>
+      <c r="G78">
+        <f>'Sheet 2'!C3144</f>
+        <v>9728</v>
+      </c>
+      <c r="H78" t="s">
+        <v>1808</v>
+      </c>
+      <c r="I78">
+        <f>'Sheet 2'!C3331</f>
+        <v>5742</v>
+      </c>
+      <c r="J78" t="s">
+        <v>1662</v>
+      </c>
+      <c r="K78">
+        <f>'Sheet 2'!C3477</f>
+        <v>1710</v>
+      </c>
+      <c r="L78" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M78">
+        <f>'Sheet 2'!C3753</f>
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" s="9" customFormat="1">
+      <c r="A79" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="10">
         <v>25941</v>
       </c>
-      <c r="C79" t="s">
-        <v>5158</v>
-      </c>
-      <c r="D79" s="1" t="b">
+      <c r="C79" s="9" t="s">
+        <v>5157</v>
+      </c>
+      <c r="D79" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C79,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E79" s="5">
+      <c r="E79" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
-      <c r="A80" t="s">
+    <row r="80" spans="1:13" s="9" customFormat="1">
+      <c r="A80" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="10">
         <v>25414</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D80" s="1" t="b">
+      <c r="D80" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C80,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E80" s="5">
+      <c r="E80" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
-      <c r="A81" t="s">
+    <row r="81" spans="1:11" s="9" customFormat="1">
+      <c r="A81" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="10">
         <v>25388</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D81" s="1" t="b">
+      <c r="D81" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C81,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E81" s="5">
+      <c r="E81" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
-      <c r="A82" t="s">
+    <row r="82" spans="1:11" s="9" customFormat="1">
+      <c r="A82" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B82" s="10">
         <v>25115</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D82" s="1" t="b">
+      <c r="D82" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C82,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E82" s="5">
+      <c r="E82" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:11">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -18077,10 +18267,24 @@
       </c>
       <c r="E83" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
+        <v>79196</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1311</v>
+      </c>
+      <c r="G83">
+        <f>'Sheet 2'!C3828</f>
+        <v>75655</v>
+      </c>
+      <c r="H83" t="s">
+        <v>2469</v>
+      </c>
+      <c r="I83">
+        <f>'Sheet 2'!C2670</f>
+        <v>3541</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -18096,10 +18300,17 @@
       </c>
       <c r="E84" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
+        <v>251705</v>
+      </c>
+      <c r="F84" t="s">
+        <v>2883</v>
+      </c>
+      <c r="G84">
+        <f>'Sheet 2'!C2256</f>
+        <v>251705</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -18115,29 +18326,36 @@
       </c>
       <c r="E85" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" t="s">
+        <v>64589</v>
+      </c>
+      <c r="F85" t="s">
+        <v>2417</v>
+      </c>
+      <c r="G85">
+        <f>'Sheet 2'!C2722</f>
+        <v>64589</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" s="9" customFormat="1">
+      <c r="A86" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B86" s="10">
         <v>23844</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="9" t="s">
         <v>5144</v>
       </c>
-      <c r="D86" s="1" t="b">
+      <c r="D86" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C86,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E86" s="5">
+      <c r="E86" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:11">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -18153,10 +18371,28 @@
       </c>
       <c r="E87" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
+        <v>17813</v>
+      </c>
+      <c r="F87" t="s">
+        <v>3335</v>
+      </c>
+      <c r="G87">
+        <f>'Sheet 2'!$C$1804</f>
+        <v>17462</v>
+      </c>
+      <c r="H87" t="s">
+        <v>3280</v>
+      </c>
+      <c r="I87">
+        <f>'Sheet 2'!$C$1859</f>
+        <v>351</v>
+      </c>
+      <c r="J87" s="8" t="s">
+        <v>5164</v>
+      </c>
+      <c r="K87" s="8"/>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -18172,10 +18408,17 @@
       </c>
       <c r="E88" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
+        <v>2673</v>
+      </c>
+      <c r="F88" t="s">
+        <v>4764</v>
+      </c>
+      <c r="G88">
+        <f>'Sheet 2'!C375</f>
+        <v>2673</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -18191,29 +18434,43 @@
       </c>
       <c r="E89" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90" t="s">
+        <v>24050</v>
+      </c>
+      <c r="F89" t="s">
+        <v>3238</v>
+      </c>
+      <c r="G89">
+        <f>'Sheet 2'!C1901</f>
+        <v>19041</v>
+      </c>
+      <c r="H89" t="s">
+        <v>4527</v>
+      </c>
+      <c r="I89">
+        <f>'Sheet 2'!C612</f>
+        <v>5009</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" s="9" customFormat="1">
+      <c r="A90" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B90" s="10">
         <v>22576</v>
       </c>
-      <c r="C90" t="s">
-        <v>5148</v>
-      </c>
-      <c r="D90" s="1" t="b">
+      <c r="C90" s="9" t="s">
+        <v>5147</v>
+      </c>
+      <c r="D90" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C90,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E90" s="5">
+      <c r="E90" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:11">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -18229,10 +18486,17 @@
       </c>
       <c r="E91" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+        <v>27738</v>
+      </c>
+      <c r="F91" t="s">
+        <v>770</v>
+      </c>
+      <c r="G91">
+        <f>'Sheet 2'!C4369</f>
+        <v>27738</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -18240,7 +18504,7 @@
         <v>22340</v>
       </c>
       <c r="C92" t="s">
-        <v>92</v>
+        <v>3854</v>
       </c>
       <c r="D92" s="1" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C92,'Sheet 2'!B:B)))&gt;0</f>
@@ -18248,10 +18512,17 @@
       </c>
       <c r="E92" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
+        <v>319</v>
+      </c>
+      <c r="F92" t="s">
+        <v>3854</v>
+      </c>
+      <c r="G92">
+        <f>'Sheet 2'!C1285</f>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -18267,67 +18538,74 @@
       </c>
       <c r="E93" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94" t="s">
+        <v>737</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>3170</v>
+      </c>
+      <c r="G93" s="6">
+        <f>'Sheet 2'!C1969</f>
+        <v>737</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" s="9" customFormat="1">
+      <c r="A94" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B94" s="10">
         <v>22132</v>
       </c>
-      <c r="C94" t="s">
-        <v>5149</v>
-      </c>
-      <c r="D94" s="1" t="b">
+      <c r="C94" s="9" t="s">
+        <v>5148</v>
+      </c>
+      <c r="D94" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C94,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E94" s="5">
+      <c r="E94" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
-      <c r="A95" t="s">
+    <row r="95" spans="1:11" s="9" customFormat="1">
+      <c r="A95" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="10">
         <v>21610</v>
       </c>
-      <c r="C95" t="s">
-        <v>5150</v>
-      </c>
-      <c r="D95" s="1" t="b">
+      <c r="C95" s="9" t="s">
+        <v>5149</v>
+      </c>
+      <c r="D95" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C95,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E95" s="5">
+      <c r="E95" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
-      <c r="A96" t="s">
+    <row r="96" spans="1:11" s="9" customFormat="1">
+      <c r="A96" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="10">
         <v>21582</v>
       </c>
-      <c r="C96" t="s">
-        <v>5151</v>
-      </c>
-      <c r="D96" s="1" t="b">
+      <c r="C96" s="9" t="s">
+        <v>5150</v>
+      </c>
+      <c r="D96" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C96,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E96" s="5">
+      <c r="E96" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:13">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -18343,29 +18621,36 @@
       </c>
       <c r="E97" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98" t="s">
+        <v>25530</v>
+      </c>
+      <c r="F97" t="s">
+        <v>3226</v>
+      </c>
+      <c r="G97">
+        <f>'Sheet 2'!C1913</f>
+        <v>25530</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" s="9" customFormat="1">
+      <c r="A98" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B98" s="10">
         <v>21405</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="9" t="s">
         <v>5144</v>
       </c>
-      <c r="D98" s="1" t="b">
+      <c r="D98" s="11" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C98,'Sheet 2'!B:B)))&gt;0</f>
         <v>0</v>
       </c>
-      <c r="E98" s="5">
+      <c r="E98" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:13">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -18381,10 +18666,38 @@
       </c>
       <c r="E99" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
+        <v>19119</v>
+      </c>
+      <c r="F99" t="s">
+        <v>693</v>
+      </c>
+      <c r="G99">
+        <f>'Sheet 2'!C4446</f>
+        <v>18800</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>1515</v>
+      </c>
+      <c r="I99" s="6">
+        <f>'Sheet 2'!C3624</f>
+        <v>35</v>
+      </c>
+      <c r="J99" s="6" t="s">
+        <v>1972</v>
+      </c>
+      <c r="K99" s="6">
+        <f>'Sheet 2'!C3167</f>
+        <v>70</v>
+      </c>
+      <c r="L99" s="6" t="s">
+        <v>2900</v>
+      </c>
+      <c r="M99" s="6">
+        <f>'Sheet 2'!C2239</f>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -18392,7 +18705,7 @@
         <v>20966</v>
       </c>
       <c r="C100" t="s">
-        <v>5152</v>
+        <v>5151</v>
       </c>
       <c r="D100" s="1" t="b">
         <f>SUMPRODUCT(--ISNUMBER(SEARCH(C100,'Sheet 2'!B:B)))&gt;0</f>
@@ -18400,10 +18713,17 @@
       </c>
       <c r="E100" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
+        <v>29507</v>
+      </c>
+      <c r="F100" t="s">
+        <v>2778</v>
+      </c>
+      <c r="G100">
+        <f>'Sheet 2'!C2361</f>
+        <v>29507</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
       <c r="A101" t="s">
         <v>101</v>
       </c>
@@ -18419,10 +18739,40 @@
       </c>
       <c r="E101" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>870</v>
+      </c>
+      <c r="F101" t="s">
+        <v>3364</v>
+      </c>
+      <c r="G101">
+        <f>'Sheet 2'!C1775</f>
+        <v>870</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
+      <c r="A104" s="14" t="s">
+        <v>5166</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
+      <c r="A105" s="15" t="s">
+        <v>5167</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13">
+      <c r="A106" s="13" t="s">
+        <v>5168</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13">
+      <c r="A107" s="16" t="s">
+        <v>5169</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J87:K87"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -18432,8 +18782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8AE58EF-29CB-4E77-BE94-4EC30FE7445D}">
   <dimension ref="A1:C5037"/>
   <sheetViews>
-    <sheetView topLeftCell="A1999" workbookViewId="0">
-      <selection activeCell="B2026" sqref="B2026"/>
+    <sheetView topLeftCell="A1748" workbookViewId="0">
+      <selection activeCell="B1775" sqref="B1775"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4"/>

</xml_diff>